<commit_message>
Update only on excel
</commit_message>
<xml_diff>
--- a/Best results_allCases.xlsx
+++ b/Best results_allCases.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gimdongchan/Documents/GitHub/quantum-flakiness-ml/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E2A0DC-6CED-3F45-809E-76DD928B7029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="1260" yWindow="12920" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="73">
   <si>
     <t>표 1</t>
   </si>
@@ -202,24 +212,83 @@
   <si>
     <t>설명</t>
   </si>
+  <si>
+    <t>eqal KNN</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>extKNN</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5fold</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5-fold</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-fold</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqlSVM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>extSVM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqlNaive Bayes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>extNaive Bayes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'alpha': 0.01}</t>
+  </si>
+  <si>
+    <t>eqlXGBoost</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>extXGB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqlRandom Forest</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>extRandom Forest</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eql Decision Tree</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>extDecisionTree</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqlDecision Tree</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="15"/>
@@ -236,6 +305,36 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="나눔명조"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,7 +344,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -268,68 +367,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -531,7 +726,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -549,7 +744,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -578,7 +773,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -603,7 +798,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -628,7 +823,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -653,7 +848,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -678,7 +873,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -703,7 +898,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -728,7 +923,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -753,7 +948,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -778,7 +973,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -791,9 +986,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -810,7 +1011,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -828,7 +1029,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -853,7 +1054,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -878,7 +1079,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -903,7 +1104,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -928,7 +1129,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +1154,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -978,7 +1179,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1003,7 +1204,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1028,7 +1229,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1053,7 +1254,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1066,9 +1267,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1082,7 +1289,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1100,7 +1307,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1129,7 +1336,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1154,7 +1361,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1179,7 +1386,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1204,7 +1411,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1229,7 +1436,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1254,7 +1461,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1486,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1304,7 +1511,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1536,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1342,941 +1549,1519 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="A27" zoomScale="175" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.1719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3984" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1172" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.2344" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="95" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="19" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s" s="3">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s" s="3">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s" s="3">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="3">
+    <row r="4" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5">
-        <v>0.766081871345029</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.783174603174603</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.746666666666667</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.755583566760037</v>
-      </c>
-      <c r="G4" t="s" s="3">
+      <c r="C4" s="4">
+        <v>0.76608187134502903</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.78317460317460297</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.74666666666666703</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.75558356676003702</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="3">
+    <row r="5" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
-        <v>0.7661290322580649</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.793956043956044</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.723611111111111</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.756349206349206</v>
-      </c>
-      <c r="G5" t="s" s="3">
+      <c r="C5" s="4">
+        <v>0.76612903225806495</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.79395604395604402</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.72361111111111098</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.75634920634920599</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="3">
+    <row r="6" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.7666666666666671</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C6" s="4">
+        <v>0.76666666666666705</v>
+      </c>
+      <c r="D6" s="4">
         <v>0.809096459096459</v>
       </c>
-      <c r="E6" s="5">
-        <v>0.731111111111111</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.7523945335710041</v>
-      </c>
-      <c r="G6" t="s" s="3">
+      <c r="E6" s="4">
+        <v>0.73111111111111104</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.75239453357100405</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="3">
+    <row r="7" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5">
-        <v>0.7563844086021509</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.781313131313131</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.7041666666666671</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.735165272799682</v>
-      </c>
-      <c r="G7" t="s" s="3">
+      <c r="C7" s="4">
+        <v>0.75638440860215095</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.78131313131313096</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.70416666666666705</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.73516527279968202</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="3">
+    <row r="8" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
-        <v>0.776608187134503</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.79531746031746</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.768888888888889</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.773818860877684</v>
-      </c>
-      <c r="G8" t="s" s="3">
+      <c r="C8" s="4">
+        <v>0.77660818713450297</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.79531746031745998</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.76888888888888896</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.77381886087768403</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="3">
+    <row r="9" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5">
-        <v>0.7758736559139791</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="C9" s="4">
+        <v>0.77587365591397905</v>
+      </c>
+      <c r="D9" s="4">
         <v>0.834733893557423</v>
       </c>
-      <c r="E9" s="5">
-        <v>0.723611111111111</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.767438271604938</v>
-      </c>
-      <c r="G9" t="s" s="3">
+      <c r="E9" s="4">
+        <v>0.72361111111111098</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.76743827160493805</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="3">
+    <row r="10" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5">
-        <v>0.755555555555556</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.788986013986014</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.7666666666666671</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.7562481962481959</v>
-      </c>
-      <c r="G10" t="s" s="3">
+      <c r="C10" s="4">
+        <v>0.75555555555555598</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.78898601398601398</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.76666666666666705</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.75624819624819595</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="3">
+    <row r="11" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s" s="3">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5">
-        <v>0.755040322580645</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.761664261664262</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="C11" s="4">
+        <v>0.75504032258064502</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.76166426166426204</v>
+      </c>
+      <c r="E11" s="4">
         <v>0.8125</v>
       </c>
-      <c r="F11" s="5">
-        <v>0.7538738738738739</v>
-      </c>
-      <c r="G11" t="s" s="3">
+      <c r="F11" s="4">
+        <v>0.75387387387387395</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" t="s" s="3">
+    <row r="12" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s" s="3">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5">
-        <v>0.851461988304094</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.873333333333333</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.8496198830409361</v>
-      </c>
-      <c r="G12" t="s" s="3">
+      <c r="C12" s="4">
+        <v>0.85146198830409403</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.87333333333333296</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.84961988304093605</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" t="s" s="3">
+    <row r="13" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s" s="3">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
-        <v>0.8081317204301079</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.826646556058321</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.786111111111111</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.803134796238245</v>
-      </c>
-      <c r="G13" t="s" s="3">
+      <c r="C13" s="4">
+        <v>0.80813172043010795</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.82664655605832105</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.78611111111111098</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.80313479623824502</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" t="s" s="3">
+    <row r="14" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s" s="3">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
-        <v>0.767836257309942</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.757222222222222</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.795555555555556</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0.770760233918129</v>
-      </c>
-      <c r="G14" t="s" s="3">
+      <c r="C14" s="4">
+        <v>0.76783625730994198</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.75722222222222202</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.79555555555555602</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.77076023391812898</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" t="s" s="3">
+    <row r="15" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s" s="3">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5">
-        <v>0.744959677419355</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.7464052287581699</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.743055555555556</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0.744216357119583</v>
-      </c>
-      <c r="G15" t="s" s="3">
+      <c r="C15" s="4">
+        <v>0.74495967741935498</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.74640522875816995</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.74305555555555602</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.74421635711958301</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" t="s" s="3">
+    <row r="16" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" t="s" s="3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s" s="3">
+      <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="5">
-        <v>0.842857142857143</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.878787878787879</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="C17" s="4">
+        <v>0.84285714285714297</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.87878787878787901</v>
+      </c>
+      <c r="E17" s="4">
         <v>0.66</v>
       </c>
-      <c r="F17" s="5">
-        <v>0.719047619047619</v>
-      </c>
-      <c r="G17" t="s" s="3">
+      <c r="F17" s="4">
+        <v>0.71904761904761905</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" t="s" s="3">
+    <row r="18" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s" s="3">
+      <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="5">
-        <v>0.778600061671292</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.68106162843005</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0.6375</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0.652380952380952</v>
-      </c>
-      <c r="G18" t="s" s="3">
+      <c r="C18" s="4">
+        <v>0.77860006167129203</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.68106162843005003</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.65238095238095195</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" t="s" s="3">
+    <row r="19" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s" s="3">
+      <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="5">
-        <v>0.778600061671292</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.68106162843005</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0.6375</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0.652380952380952</v>
-      </c>
-      <c r="G19" t="s" s="3">
+      <c r="C19" s="4">
+        <v>0.77860006167129203</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.68106162843005003</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.65238095238095195</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" t="s" s="3">
+    <row r="20" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s" s="3">
+      <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="5">
-        <v>0.828571428571429</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="C20" s="4">
+        <v>0.82857142857142896</v>
+      </c>
+      <c r="D20" s="4">
         <v>0.817676767676768</v>
       </c>
-      <c r="E20" s="5">
-        <v>0.6644444444444439</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0.716746031746032</v>
-      </c>
-      <c r="G20" t="s" s="3">
+      <c r="E20" s="4">
+        <v>0.66444444444444395</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.71674603174603202</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" t="s" s="3">
+    <row r="21" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s" s="3">
+      <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="5">
-        <v>0.843200740055504</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.838888888888889</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0.661111111111111</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0.734797659528843</v>
-      </c>
-      <c r="G21" t="s" s="3">
+      <c r="C21" s="4">
+        <v>0.84320074005550405</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.83888888888888902</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.66111111111111098</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.73479765952884302</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" t="s" s="3">
+    <row r="22" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s" s="3">
+      <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="5">
-        <v>0.885714285714286</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0.764069264069264</v>
-      </c>
-      <c r="E22" s="5">
-        <v>0.955555555555556</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0.848484848484848</v>
-      </c>
-      <c r="G22" t="s" s="3">
+      <c r="C22" s="4">
+        <v>0.88571428571428601</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.76406926406926401</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.95555555555555605</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.84848484848484795</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" t="s" s="3">
+    <row r="23" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B23" t="s" s="3">
+      <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="5">
-        <v>0.878199198273204</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0.74534821903243</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0.977777777777778</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0.844722918407129</v>
-      </c>
-      <c r="G23" t="s" s="3">
+      <c r="C23" s="4">
+        <v>0.87819919827320403</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.74534821903242998</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.97777777777777797</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.84472291840712899</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" t="s" s="3">
+    <row r="24" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" t="s" s="3">
+      <c r="B24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="5">
-        <v>0.8071428571428571</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0.794444444444444</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0.593333333333333</v>
-      </c>
-      <c r="F24" s="5">
+      <c r="C24" s="4">
+        <v>0.80714285714285705</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.79444444444444395</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.59333333333333305</v>
+      </c>
+      <c r="F24" s="4">
         <v>0.66600089968511</v>
       </c>
-      <c r="G24" t="s" s="3">
+      <c r="G24" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" t="s" s="3">
+    <row r="25" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s" s="3">
+      <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="5">
-        <v>0.835800185013876</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0.744876898127672</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0.786111111111111</v>
-      </c>
-      <c r="F25" s="5">
+      <c r="C25" s="4">
+        <v>0.83580018501387598</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.74487689812767199</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.78611111111111098</v>
+      </c>
+      <c r="F25" s="4">
         <v>0.763118873463701</v>
       </c>
-      <c r="G25" t="s" s="3">
+      <c r="G25" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" t="s" s="3">
+    <row r="26" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s" s="3">
+      <c r="B26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="5">
-        <v>0.835714285714286</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0.849350649350649</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0.6466666666666669</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0.711932773109244</v>
-      </c>
-      <c r="G26" t="s" s="3">
+      <c r="C26" s="4">
+        <v>0.83571428571428596</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.84935064935064897</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.64666666666666694</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.71193277310924397</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" ht="13.55" customHeight="1">
-      <c r="A27" t="s" s="3">
+    <row r="27" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="s" s="3">
+      <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="5">
-        <v>0.849984582176997</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0.885714285714286</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0.6375</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0.737435897435898</v>
-      </c>
-      <c r="G27" t="s" s="3">
+      <c r="C27" s="4">
+        <v>0.84998458217699702</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.88571428571428601</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.73743589743589799</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" t="s" s="3">
+    <row r="28" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s" s="3">
+      <c r="B28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="5">
-        <v>0.828571428571429</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0.758297258297258</v>
-      </c>
-      <c r="E28" s="5">
-        <v>0.746666666666667</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0.748496240601504</v>
-      </c>
-      <c r="G28" t="s" s="3">
+      <c r="C28" s="4">
+        <v>0.82857142857142896</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.75829725829725803</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.74666666666666703</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.74849624060150399</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" t="s" s="3">
+    <row r="29" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="s" s="3">
+      <c r="B29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="5">
-        <v>0.792938637064446</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0.6890756302521009</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0.701388888888889</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0.6945315221177289</v>
-      </c>
-      <c r="G29" t="s" s="3">
+      <c r="C29" s="4">
+        <v>0.79293863706444601</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.68907563025210095</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.70138888888888895</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.69453152211772895</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" ht="13.55" customHeight="1">
-      <c r="A30" t="s" s="3">
+    <row r="30" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" t="s" s="3">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B31" t="s" s="3">
+      <c r="B31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" t="s" s="3">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" ht="24.65" customHeight="1">
-      <c r="A32" t="s" s="3">
+    <row r="32" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>3</v>
       </c>
-      <c r="C32" s="6">
-        <v>0.840548340548341</v>
-      </c>
-      <c r="D32" s="6">
-        <v>0.518518518518519</v>
-      </c>
-      <c r="E32" s="6">
-        <v>0.447222222222222</v>
-      </c>
-      <c r="F32" s="6">
-        <v>0.474747474747475</v>
-      </c>
-      <c r="G32" t="s" s="8">
+      <c r="C32" s="5">
+        <v>0.84054834054834104</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.51851851851851904</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0.44722222222222202</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0.47474747474747497</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" ht="24.65" customHeight="1">
-      <c r="A33" t="s" s="3">
+    <row r="33" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <v>5</v>
       </c>
-      <c r="C33" s="5">
-        <v>0.854237288135593</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0.553571428571429</v>
-      </c>
-      <c r="E33" s="5">
-        <v>0.535555555555556</v>
-      </c>
-      <c r="F33" s="5">
-        <v>0.533800186741363</v>
-      </c>
-      <c r="G33" t="s" s="8">
+      <c r="C33" s="4">
+        <v>0.85423728813559296</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.55357142857142905</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.53555555555555601</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0.53380018674136298</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" ht="24.65" customHeight="1">
-      <c r="A34" t="s" s="3">
+    <row r="34" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>3</v>
       </c>
-      <c r="C34" s="5">
-        <v>0.867896653610939</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0.613553113553114</v>
-      </c>
-      <c r="E34" s="5">
-        <v>0.388888888888889</v>
-      </c>
-      <c r="F34" s="5">
+      <c r="C34" s="4">
+        <v>0.86789665361093904</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.61355311355311404</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0.38888888888888901</v>
+      </c>
+      <c r="F34" s="4">
         <v>0.465148378191856</v>
       </c>
-      <c r="G34" t="s" s="8">
+      <c r="G34" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" ht="24.65" customHeight="1">
-      <c r="A35" t="s" s="3">
+    <row r="35" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>5</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>0.884745762711865</v>
       </c>
-      <c r="D35" s="5">
-        <v>0.726428571428571</v>
-      </c>
-      <c r="E35" s="5">
-        <v>0.446666666666667</v>
-      </c>
-      <c r="F35" s="5">
-        <v>0.544537815126051</v>
-      </c>
-      <c r="G35" t="s" s="8">
+      <c r="D35" s="4">
+        <v>0.72642857142857098</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0.44666666666666699</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0.54453781512605104</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" ht="24.65" customHeight="1">
-      <c r="A36" t="s" s="3">
+    <row r="36" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>3</v>
       </c>
-      <c r="C36" s="5">
-        <v>0.911908197622483</v>
-      </c>
-      <c r="D36" s="5">
-        <v>0.785576923076923</v>
-      </c>
-      <c r="E36" s="5">
-        <v>0.638888888888889</v>
-      </c>
-      <c r="F36" s="5">
-        <v>0.698031135531136</v>
-      </c>
-      <c r="G36" t="s" s="8">
+      <c r="C36" s="4">
+        <v>0.91190819762248299</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.78557692307692295</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.69803113553113605</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" ht="24.65" customHeight="1">
-      <c r="A37" t="s" s="3">
+    <row r="37" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>5</v>
       </c>
-      <c r="C37" s="5">
-        <v>0.932203389830508</v>
-      </c>
-      <c r="D37" s="5">
-        <v>0.777121212121212</v>
-      </c>
-      <c r="E37" s="5">
-        <v>0.806666666666667</v>
-      </c>
-      <c r="F37" s="5">
-        <v>0.787700534759358</v>
-      </c>
-      <c r="G37" t="s" s="8">
+      <c r="C37" s="4">
+        <v>0.93220338983050799</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.77712121212121199</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0.80666666666666698</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0.78770053475935797</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" ht="24.65" customHeight="1">
-      <c r="A38" t="s" s="3">
+    <row r="38" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>3</v>
       </c>
-      <c r="C38" s="5">
-        <v>0.884766027623171</v>
-      </c>
-      <c r="D38" s="5">
-        <v>0.902777777777778</v>
-      </c>
-      <c r="E38" s="5">
-        <v>0.322222222222222</v>
-      </c>
-      <c r="F38" s="5">
-        <v>0.459676860134526</v>
-      </c>
-      <c r="G38" t="s" s="8">
+      <c r="C38" s="4">
+        <v>0.88476602762317103</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.90277777777777801</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.32222222222222202</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0.45967686013452602</v>
+      </c>
+      <c r="G38" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" ht="24.65" customHeight="1">
-      <c r="A39" t="s" s="3">
-        <v>49</v>
-      </c>
-      <c r="B39" s="5">
+    <row r="40" spans="1:7" ht="76.75" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="4">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.88483474197759904</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.73106060606060597</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0.42916666666666697</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0.53632478632478597</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="112.75" customHeight="1">
+      <c r="A41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="4">
         <v>5</v>
       </c>
-      <c r="C39" s="5">
-        <v>0.894915254237288</v>
-      </c>
-      <c r="D39" s="5">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5">
-        <v>0.337777777777778</v>
-      </c>
-      <c r="F39" s="5">
-        <v>0.488717948717949</v>
-      </c>
-      <c r="G39" t="s" s="8">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" ht="76.7" customHeight="1">
-      <c r="A40" t="s" s="3">
-        <v>52</v>
-      </c>
-      <c r="B40" s="5">
-        <v>3</v>
-      </c>
-      <c r="C40" s="5">
-        <v>0.884834741977599</v>
-      </c>
-      <c r="D40" s="5">
-        <v>0.731060606060606</v>
-      </c>
-      <c r="E40" s="5">
-        <v>0.429166666666667</v>
-      </c>
-      <c r="F40" s="5">
-        <v>0.536324786324786</v>
-      </c>
-      <c r="G40" t="s" s="8">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" ht="112.65" customHeight="1">
-      <c r="A41" t="s" s="3">
-        <v>52</v>
-      </c>
-      <c r="B41" s="5">
-        <v>5</v>
-      </c>
-      <c r="C41" s="5">
-        <v>0.894915254237288</v>
-      </c>
-      <c r="D41" s="5">
-        <v>0.803333333333333</v>
-      </c>
-      <c r="E41" s="5">
+      <c r="C41" s="4">
+        <v>0.89491525423728802</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.80333333333333301</v>
+      </c>
+      <c r="E41" s="4">
         <v>0.448888888888889</v>
       </c>
-      <c r="F41" s="5">
-        <v>0.572307692307692</v>
-      </c>
-      <c r="G41" t="s" s="8">
+      <c r="F41" s="4">
+        <v>0.57230769230769196</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" ht="26.45" customHeight="1">
-      <c r="A42" t="s" s="9">
+    <row r="42" spans="1:7" ht="26.5" customHeight="1">
+      <c r="A42" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A42:G42"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9A8C2F-33D0-774D-8B8F-F31E2D57CC2B}">
+  <dimension ref="A2:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="200" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.76612903225806495</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.79395604395604402</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.72361111111111098</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.75634920634920599</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="14" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.86789665361093904</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.61355311355311404</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.38888888888888901</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.465148378191856</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.76608187134502903</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.78317460317460297</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.74666666666666703</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.75558356676003702</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.884745762711865</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.72642857142857098</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.44666666666666699</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.54453781512605104</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.75638440860215095</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.78131313131313096</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.70416666666666705</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.73516527279968202</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.90507111935683404</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.82828282828282795</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.49305555555555602</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.61010101010101003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.76666666666666705</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.809096459096459</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.73111111111111104</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.75239453357100405</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.91186440677966096</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.82642857142857096</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.55333333333333301</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.65793650793650804</v>
+      </c>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.77587365591397905</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.834733893557423</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.72361111111111098</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.76743827160493805</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="12" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.91190819762248299</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.78557692307692295</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.69803113553113605</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.77660818713450297</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.79531746031745998</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.76888888888888896</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.77381886087768403</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.93220338983050799</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.77712121212121199</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.80666666666666698</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.78770053475935797</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0.75504032300000001</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0.76166426200000004</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.8125</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.75387387400000005</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.88483474197759904</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.73106060606060597</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.42916666666666697</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.53632478632478597</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A17" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.75555555555555598</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.78898601398601398</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.76666666666666705</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.75624819624819595</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.89491525423728802</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.80333333333333301</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.448888888888889</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.57230769230769196</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.80813172043010795</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.82664655605832105</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.78611111111111098</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.80313479623824502</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.88476602762317103</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.90277777777777801</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.32222222222222202</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.45967686013452602</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.85146198830409403</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.87333333333333296</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.84961988304093605</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="14" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.89491525423728802</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.33777777777777801</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.48871794871794899</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.74495967741935498</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.74640522875816995</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.74305555555555602</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.74421635711958301</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.84054834054834104</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.51851851851851904</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.44722222222222202</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.47474747474747497</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.76783625730994198</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.75722222222222202</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.79555555555555602</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.77076023391812898</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="13" customHeight="1">
+      <c r="A26" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="17">
+        <v>0.85423728799999998</v>
+      </c>
+      <c r="D26" s="17">
+        <v>0.553571429</v>
+      </c>
+      <c r="E26" s="17">
+        <v>0.53555555600000004</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0.53380018699999998</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>